<commit_message>
Objetivos, Solucion, Actividades, Presupuesto
</commit_message>
<xml_diff>
--- a/SEMINARIO_DE_GRADO/PRESUPUESTO/Presupuesto.xlsx
+++ b/SEMINARIO_DE_GRADO/PRESUPUESTO/Presupuesto.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\GITHUB\PRESBYOPIA\SEMINARIO_DE_GRADO\PRESUPUESTO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3526BEB7-38B6-4D64-97E9-B63C641ECBFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6777F97A-81FE-4013-BC6A-C4905FBAC05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
   <si>
     <t>Recursos</t>
   </si>
@@ -122,9 +122,6 @@
     <t>Persona</t>
   </si>
   <si>
-    <t>Semanas de Trabajo</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -141,6 +138,12 @@
   </si>
   <si>
     <t>Costo total Poyecto</t>
+  </si>
+  <si>
+    <t>Horas de trabajo del Cliente</t>
+  </si>
+  <si>
+    <t>Semanas</t>
   </si>
 </sst>
 </file>
@@ -347,16 +350,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -368,20 +364,26 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="13" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -391,23 +393,32 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -418,17 +429,11 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -711,16 +716,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection sqref="A1:F24"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="88" workbookViewId="0">
+      <selection activeCell="F25" sqref="A1:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
@@ -728,54 +733,54 @@
     <col min="8" max="8" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="20" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>4000000</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <f>C3/4</f>
         <v>1000000</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="5">
+      <c r="E3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="4">
         <f>D3</f>
         <v>1000000</v>
       </c>
@@ -784,19 +789,19 @@
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>2500000</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <f>C4</f>
         <v>2500000</v>
       </c>
@@ -805,19 +810,19 @@
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>157000</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <f t="shared" ref="F5:F6" si="0">C5</f>
         <v>157000</v>
       </c>
@@ -826,19 +831,19 @@
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>1</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>100000</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
@@ -847,20 +852,20 @@
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>1</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>15000000</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <f>C7/4</f>
         <v>3750000</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="5">
+      <c r="E7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="4">
         <f>D7</f>
         <v>3750000</v>
       </c>
@@ -869,19 +874,19 @@
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>1</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>350000</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <f>C8</f>
         <v>350000</v>
       </c>
@@ -890,19 +895,19 @@
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>5</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>100000</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <f t="shared" ref="F9:F10" si="1">C9</f>
         <v>100000</v>
       </c>
@@ -911,19 +916,19 @@
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>150000</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <f t="shared" si="1"/>
         <v>150000</v>
       </c>
@@ -932,20 +937,20 @@
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>2</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>10000000</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <f>C11/4</f>
         <v>2500000</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="5">
+      <c r="E11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="4">
         <f>D11</f>
         <v>2500000</v>
       </c>
@@ -954,232 +959,253 @@
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>1</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>200000</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <f>C12</f>
         <v>200000</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>1</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>100000</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <f t="shared" ref="F13:F14" si="2">C13</f>
         <v>100000</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>1</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>100000</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <f t="shared" si="2"/>
         <v>100000</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="9">
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="29"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="6">
         <f>SUM(F3:F14)</f>
         <v>11007000</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="38"/>
+      <c r="A16" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="34"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="8">
         <v>1</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="9">
         <v>20000000</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="11" t="s">
+      <c r="D17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="10">
         <f>C17</f>
         <v>20000000</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="35"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="37"/>
     </row>
     <row r="19" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="27" t="s">
+      <c r="B19" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="32" t="s">
+      <c r="F19" s="22" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B20" s="12">
         <v>34</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="12">
         <v>5</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="13">
         <v>160000</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="14">
         <f>D20*C20*B20</f>
         <v>27200000</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="14" t="s">
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="12">
+        <v>34</v>
+      </c>
+      <c r="C21" s="12">
+        <v>4</v>
+      </c>
+      <c r="D21" s="13">
+        <v>160000</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="14">
+        <f t="shared" ref="F21" si="3">D21*C21*B21</f>
+        <v>21760000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B22" s="12">
         <v>34</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C22" s="12">
         <v>2</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D22" s="13">
         <v>160000</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E22" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F21" s="17">
-        <f t="shared" ref="F21:F22" si="3">D21*C21*B21</f>
+      <c r="F22" s="14">
+        <f t="shared" ref="F22:F23" si="4">D22*C22*B22</f>
         <v>10880000</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="14" t="s">
+    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B23" s="12">
         <v>34</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C23" s="12">
         <v>15</v>
       </c>
-      <c r="D22" s="16">
+      <c r="D23" s="13">
         <v>60000</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E23" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="17">
-        <f t="shared" si="3"/>
+      <c r="F23" s="14">
+        <f t="shared" si="4"/>
         <v>30600000</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="14" t="s">
+    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="26"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="15">
+        <f>F17+F20+F22+F23</f>
+        <v>88680000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="21">
-        <f>F17+F20+F21+F22</f>
-        <v>88680000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="23">
-        <f>F23+F15</f>
+      <c r="B25" s="23"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="17">
+        <f>F24+F15</f>
         <v>99687000</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B25:E25"/>
     <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B23:E23"/>
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A16:F16"/>

</xml_diff>